<commit_message>
Atualização da Conferência LN - EST
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_EST.xlsx
+++ b/Documentação/Planilhas/Conferencia_EST.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="stg_est_crossdocking" sheetId="95" r:id="rId1"/>
-    <sheet name="stg_est_referencia" sheetId="103" r:id="rId2"/>
-    <sheet name="Plan1" sheetId="102" r:id="rId3"/>
+    <sheet name="stg_est_referencia" sheetId="105" r:id="rId2"/>
+    <sheet name="stg_est_estoque" sheetId="107" r:id="rId3"/>
+    <sheet name="Plan1" sheetId="102" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="167">
   <si>
     <t>1</t>
   </si>
@@ -58,9 +59,6 @@
   </si>
   <si>
     <t>CD_TIPO_NF</t>
-  </si>
-  <si>
-    <t>5000.0000</t>
   </si>
   <si>
     <t>ULTIMA_ATUALIZ_NF</t>
@@ -241,15 +239,6 @@
     <t>13422907</t>
   </si>
   <si>
-    <t>-1000.0000</t>
-  </si>
-  <si>
-    <t>2014-07-14 16:30:08.000</t>
-  </si>
-  <si>
-    <t>13422422</t>
-  </si>
-  <si>
     <t>2014-07-10 18:40:18.000</t>
   </si>
   <si>
@@ -259,12 +248,6 @@
     <t>2014-06-25 13:36:57.000</t>
   </si>
   <si>
-    <t>13422423</t>
-  </si>
-  <si>
-    <t>2014-07-11 16:20:26.000</t>
-  </si>
-  <si>
     <t>58191</t>
   </si>
   <si>
@@ -274,9 +257,6 @@
     <t>2014-06-21 19:36:46.000</t>
   </si>
   <si>
-    <t>452343</t>
-  </si>
-  <si>
     <t>Sessão tcmcs0503m000</t>
   </si>
   <si>
@@ -301,9 +281,6 @@
     <t>Pegar a informação da coluna Saldo Disponível</t>
   </si>
   <si>
-    <t>Quantidade Fornecedor - Saldo Disponível</t>
-  </si>
-  <si>
     <t>é o campo interno [rcd_utc] da tabela tznwmd200201. Não temos como conferir isso pelo LN</t>
   </si>
   <si>
@@ -427,30 +404,6 @@
     <t>R10000023</t>
   </si>
   <si>
-    <t>Pegar a informação do cód Item no cabeçalho da tela</t>
-  </si>
-  <si>
-    <t>Pegar a informação da coluna Armazém</t>
-  </si>
-  <si>
-    <t>Pegar a informação da coluna Unidade Empresarial</t>
-  </si>
-  <si>
-    <t>Fazer o detalhamento do depósito. Na aba Geral, seção Armazém de Terceiro, pegar a informação do Tipo de Armazém de Terceiro [sem preenchimento = zero]</t>
-  </si>
-  <si>
-    <t>whwmd2515m000 [na lupinha, após limpar os campos, selecionar apenas o item desejado]</t>
-  </si>
-  <si>
-    <t>Selecionar o Depósito desejado. No menu Specific, selecione Transações, Transações de Inventário. Pegar as referências existentes na coluna Recebimentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detalhar o Depósito desejado. Na aba "Datas/preços", seção "Fixar Preço", pegar a informação MAUC (por armazém)  </t>
-  </si>
-  <si>
-    <t>Para validar a Qt_Fisica, é necessário do NR_Ordem. Aproveite para pegar os mesmos nesta tela</t>
-  </si>
-  <si>
     <t>NR_ORDEM</t>
   </si>
   <si>
@@ -458,15 +411,6 @@
   </si>
   <si>
     <t>V10000005</t>
-  </si>
-  <si>
-    <t>sessão whinh3512m000</t>
-  </si>
-  <si>
-    <t>Na lupinha, informar o NR_REFERENCIA. No menu Specific, selecionar "Rec Fiscal - Resumo". Pegar a informação da coluna "Referência Fiscal"</t>
-  </si>
-  <si>
-    <t>tcmcs0503m000, tcemm0130m000, whwmd2515m000, whina1512m000 e whinh3512m000</t>
   </si>
   <si>
     <t>De posse do código da "Unidade Empresarial", ir para a sessão "tcemm0130m000"  e informar o Cód da Unidade Empresarial na coluna "Unid Empresarial". Pegar a informação da coluna "Cat da uni empresarial"</t>
@@ -476,6 +420,108 @@
 Na aba Ordem, filtrar a ordem de venda encontrada para o NR_REFERENCIA, na coluna Ordem.
 Com o filtro realizado, retornar para a aba Transações e pegar os valores da coluna "Quantidade Recebida" 
  [não é a linha que aparece como total. Temos que somar cada linha apresentada para o filtro realizado]</t>
+  </si>
+  <si>
+    <t>13423312</t>
+  </si>
+  <si>
+    <t>2014-07-24 15:58:47.000</t>
+  </si>
+  <si>
+    <t>452364</t>
+  </si>
+  <si>
+    <t>332327</t>
+  </si>
+  <si>
+    <t>Execurtar a equação: "Quantidade Fornecedor" - "Saldo Disponível"</t>
+  </si>
+  <si>
+    <t>sessão tdrecl504m00l [Na lupinha,  informar o FIRE na coluna "Referência Fiscal"]</t>
+  </si>
+  <si>
+    <t>Pegar a informação na coluna "Referência Fiscal"</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento da Referência Fiscal desejada. Na aba inferior "Linha", pegar a segunda  informação da coluna Item</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento da Referência Fiscal desejada. Na aba inferior "Linha", pedir o detalhamento do item desejado. Na aba inferior "Dados de Origem", pegar a informação da coluna Recebimento</t>
+  </si>
+  <si>
+    <t>Para validar a Qt_Fisica, é necessário do NR_Ordem. Aproveite para pegar os mesmos nesta tela [coluna Ordem]</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento da Referência Fiscal desejada. Na aba inferior "Linha", pedir o detalhamento do item desejado. Na aba superior "Outros", seção "Dados da Ordem" pegar a informação de Almoxarifado de Recebimento</t>
+  </si>
+  <si>
+    <t>Informar o CD_DEPOSITO na coluna armazem e pedir o detalhamento do mesmo. Na aba Geral, seção Armazém de Terceiro, pegar a informação do Tipo de Armazém de Terceiro [sem preenchimento = zero]</t>
+  </si>
+  <si>
+    <t>Informar o CD_DEPOSITO na coluna armazem e pedir o detalhamento do mesmo. Na aba Geral, seção Geral, pegar a informação da Unidade Empresarial</t>
+  </si>
+  <si>
+    <t>Sessão whwmd2515m000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na Lupinha, informar o CD_ITEM e CD_DEPOSITO e detalhar o Depósito desejado. Na aba "Datas/preços", seção "Fixar Preço", pegar a informação MAUC (por armazém)  </t>
+  </si>
+  <si>
+    <t>tdrecl504m00l, tcmcs0503m000, tcemm0130m000, whwmd2515m000, whina1512m000</t>
+  </si>
+  <si>
+    <t>dbo.stg_est_estoque</t>
+  </si>
+  <si>
+    <t>QT_ROMANEADA</t>
+  </si>
+  <si>
+    <t>CD_TIPO_BLOQUEIO</t>
+  </si>
+  <si>
+    <t>CD0016</t>
+  </si>
+  <si>
+    <t>ALYNE</t>
+  </si>
+  <si>
+    <t>984.0000</t>
+  </si>
+  <si>
+    <t>100.0000</t>
+  </si>
+  <si>
+    <t>N00016</t>
+  </si>
+  <si>
+    <t>WN</t>
+  </si>
+  <si>
+    <t>ALYNE_01</t>
+  </si>
+  <si>
+    <t>995.0000</t>
+  </si>
+  <si>
+    <t>ALYNE_02</t>
+  </si>
+  <si>
+    <t>50.0000</t>
+  </si>
+  <si>
+    <t>129441</t>
+  </si>
+  <si>
+    <t>32.0000</t>
+  </si>
+  <si>
+    <t>6.0000</t>
+  </si>
+  <si>
+    <t>1678964</t>
+  </si>
+  <si>
+    <t>13.0000</t>
   </si>
 </sst>
 </file>
@@ -522,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,8 +599,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -658,11 +710,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -674,6 +775,30 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -692,32 +817,62 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1027,7 +1182,7 @@
   <dimension ref="A2:AG32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1069,21 +1224,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1097,71 +1252,71 @@
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
+      <c r="E7" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="E8" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1169,25 +1324,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1195,25 +1350,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1221,22 +1376,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>75</v>
@@ -1247,25 +1402,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1273,25 +1428,25 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1299,25 +1454,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1325,25 +1480,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1351,128 +1506,128 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="11.25" customHeight="1">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="11.25" customHeight="1">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="11.25" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="G22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="12"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="12"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="12"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="C26" s="12"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="C27" s="12"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="C28" s="12"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="C29" s="12"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" s="1"/>
-      <c r="C30" s="12"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="1"/>
@@ -1482,11 +1637,7 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="H22:H25"/>
     <mergeCell ref="D19:G21"/>
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="E22:E25"/>
@@ -1494,7 +1645,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="F22:F25"/>
     <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1508,21 +1663,21 @@
   </sheetPr>
   <dimension ref="A2:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:K16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22" style="2" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="29.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="20" style="2" customWidth="1"/>
@@ -1552,21 +1707,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1574,104 +1729,104 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>108</v>
+      <c r="I7" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>111</v>
+      <c r="I8" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1679,31 +1834,31 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1711,31 +1866,31 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="I10" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1743,31 +1898,31 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1775,31 +1930,31 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1807,31 +1962,31 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1839,31 +1994,31 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="I14" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1871,31 +2026,31 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="J15" s="2" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1903,31 +2058,31 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="I16" s="2" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -1939,191 +2094,685 @@
       <c r="AH18" s="1"/>
     </row>
     <row r="19" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>147</v>
+      <c r="B19" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
     <row r="20" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B20" s="6"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="11"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
     <row r="21" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B21" s="7"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="11"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
     <row r="22" spans="1:34" ht="11.25" customHeight="1">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="C22" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>148</v>
+      <c r="E22" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" s="26" t="s">
+        <v>132</v>
       </c>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
     <row r="23" spans="1:34">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="12"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="27"/>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="12"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="27"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="12"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="27"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="12"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="27"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="I27" s="19"/>
+      <c r="J27" s="27"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="G28" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="I28" s="19"/>
+      <c r="D28" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J28" s="27"/>
     </row>
     <row r="29" spans="1:34">
-      <c r="G29" s="17"/>
-      <c r="I29" s="19"/>
+      <c r="D29" s="12"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:34">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="G30" s="17"/>
-      <c r="I30" s="19"/>
+      <c r="D30" s="12"/>
+      <c r="F30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:34">
-      <c r="I31" s="19"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:34">
-      <c r="I32" s="19"/>
-    </row>
-    <row r="33" spans="9:9">
-      <c r="I33" s="19"/>
-    </row>
-    <row r="34" spans="9:9">
-      <c r="I34" s="19"/>
+      <c r="J32" s="27"/>
+    </row>
+    <row r="33" spans="10:10">
+      <c r="J33" s="27"/>
+    </row>
+    <row r="34" spans="10:10">
+      <c r="J34" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="J22:J34"/>
+    <mergeCell ref="B19:E21"/>
+    <mergeCell ref="F19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="J19:J21"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="D19:H21"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I22:I34"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A22:A26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A2:AH16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="22" style="2" customWidth="1"/>
+    <col min="15" max="15" width="34.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="34" style="2" customWidth="1"/>
+    <col min="17" max="17" width="34.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="22.85546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="20.85546875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="23.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="2" customWidth="1"/>
+    <col min="24" max="24" width="21.140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="22.28515625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="25" style="2" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="31.42578125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="27.85546875" style="2" customWidth="1"/>
+    <col min="31" max="31" width="14.5703125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="19.5703125" style="2" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="21">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
@@ -2132,7 +2781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:F48"/>
   <sheetViews>
@@ -2171,7 +2820,7 @@
     </row>
     <row r="6" spans="3:6">
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -2198,7 +2847,7 @@
     </row>
     <row r="9" spans="3:6">
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -2207,7 +2856,7 @@
     </row>
     <row r="10" spans="3:6">
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -2216,7 +2865,7 @@
     </row>
     <row r="11" spans="3:6">
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -2225,7 +2874,7 @@
     </row>
     <row r="12" spans="3:6">
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -2234,7 +2883,7 @@
     </row>
     <row r="13" spans="3:6">
       <c r="C13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -2243,7 +2892,7 @@
     </row>
     <row r="14" spans="3:6">
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -2261,7 +2910,7 @@
     </row>
     <row r="16" spans="3:6">
       <c r="C16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -2270,7 +2919,7 @@
     </row>
     <row r="17" spans="3:6">
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -2288,7 +2937,7 @@
     </row>
     <row r="19" spans="3:6">
       <c r="C19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -2297,7 +2946,7 @@
     </row>
     <row r="20" spans="3:6">
       <c r="C20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -2306,7 +2955,7 @@
     </row>
     <row r="21" spans="3:6">
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -2315,7 +2964,7 @@
     </row>
     <row r="22" spans="3:6">
       <c r="C22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -2324,7 +2973,7 @@
     </row>
     <row r="23" spans="3:6">
       <c r="C23" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -2333,7 +2982,7 @@
     </row>
     <row r="24" spans="3:6">
       <c r="C24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -2342,7 +2991,7 @@
     </row>
     <row r="25" spans="3:6">
       <c r="C25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -2351,7 +3000,7 @@
     </row>
     <row r="26" spans="3:6">
       <c r="C26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -2360,7 +3009,7 @@
     </row>
     <row r="27" spans="3:6">
       <c r="C27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -2369,7 +3018,7 @@
     </row>
     <row r="28" spans="3:6">
       <c r="C28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -2378,7 +3027,7 @@
     </row>
     <row r="29" spans="3:6">
       <c r="C29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -2387,7 +3036,7 @@
     </row>
     <row r="30" spans="3:6">
       <c r="C30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -2396,7 +3045,7 @@
     </row>
     <row r="31" spans="3:6">
       <c r="C31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -2405,7 +3054,7 @@
     </row>
     <row r="32" spans="3:6">
       <c r="C32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -2414,7 +3063,7 @@
     </row>
     <row r="33" spans="3:6">
       <c r="C33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -2423,7 +3072,7 @@
     </row>
     <row r="34" spans="3:6">
       <c r="C34" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -2432,7 +3081,7 @@
     </row>
     <row r="35" spans="3:6">
       <c r="C35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
@@ -2441,7 +3090,7 @@
     </row>
     <row r="36" spans="3:6">
       <c r="C36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -2450,7 +3099,7 @@
     </row>
     <row r="37" spans="3:6">
       <c r="C37" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -2459,7 +3108,7 @@
     </row>
     <row r="38" spans="3:6">
       <c r="C38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -2468,7 +3117,7 @@
     </row>
     <row r="39" spans="3:6">
       <c r="C39" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
@@ -2477,7 +3126,7 @@
     </row>
     <row r="40" spans="3:6">
       <c r="C40" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
@@ -2486,7 +3135,7 @@
     </row>
     <row r="41" spans="3:6">
       <c r="C41" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -2495,7 +3144,7 @@
     </row>
     <row r="42" spans="3:6">
       <c r="C42" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -2504,7 +3153,7 @@
     </row>
     <row r="43" spans="3:6">
       <c r="C43" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -2513,7 +3162,7 @@
     </row>
     <row r="44" spans="3:6">
       <c r="C44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
@@ -2522,7 +3171,7 @@
     </row>
     <row r="45" spans="3:6">
       <c r="C45" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -2531,7 +3180,7 @@
     </row>
     <row r="46" spans="3:6">
       <c r="C46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -2540,7 +3189,7 @@
     </row>
     <row r="47" spans="3:6">
       <c r="C47" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
@@ -2549,7 +3198,7 @@
     </row>
     <row r="48" spans="3:6">
       <c r="C48" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
atualização da conferência LN - Estoque
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_EST.xlsx
+++ b/Documentação/Planilhas/Conferencia_EST.xlsx
@@ -964,6 +964,34 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -976,6 +1004,24 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1033,24 +1079,6 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1060,51 +1088,23 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1456,19 +1456,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>73</v>
       </c>
@@ -1760,106 +1760,106 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="C26" s="6"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="C27" s="6"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="C28" s="6"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="C29" s="6"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" s="1"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="1"/>
@@ -1939,19 +1939,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>139</v>
       </c>
@@ -2326,181 +2326,188 @@
       <c r="AH18" s="1"/>
     </row>
     <row r="19" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="23" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="29" t="s">
+      <c r="G19" s="40"/>
+      <c r="H19" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="I19" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="20" t="s">
         <v>48</v>
       </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
     <row r="20" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
     <row r="21" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
     <row r="22" spans="1:34" ht="11.25" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="I22" s="35" t="s">
+      <c r="I22" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="27" t="s">
         <v>123</v>
       </c>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
     <row r="23" spans="1:34">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="12"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="28"/>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="12"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="28"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="12"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="28"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="12"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="J27" s="12"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="J28" s="12"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:34" ht="33.75">
-      <c r="D29" s="10"/>
-      <c r="F29" s="41" t="s">
+      <c r="D29" s="26"/>
+      <c r="F29" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="J29" s="12"/>
+      <c r="J29" s="28"/>
     </row>
     <row r="30" spans="1:34">
-      <c r="D30" s="10"/>
+      <c r="D30" s="26"/>
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="J30" s="12"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:34">
-      <c r="J31" s="12"/>
+      <c r="J31" s="28"/>
     </row>
     <row r="32" spans="1:34">
-      <c r="J32" s="12"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="10:10">
-      <c r="J33" s="12"/>
+      <c r="J33" s="28"/>
     </row>
     <row r="34" spans="10:10">
-      <c r="J34" s="13"/>
+      <c r="J34" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="J22:J34"/>
+    <mergeCell ref="B19:E21"/>
+    <mergeCell ref="F19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="I22:I26"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="J19:J21"/>
@@ -2512,13 +2519,6 @@
     <mergeCell ref="G22:G26"/>
     <mergeCell ref="D22:D26"/>
     <mergeCell ref="B22:B26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="J22:J34"/>
-    <mergeCell ref="B19:E21"/>
-    <mergeCell ref="F19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2533,7 +2533,7 @@
   <dimension ref="A2:AI54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2576,739 +2576,739 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:35" ht="21">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="21">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="K6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="52" t="s">
+      <c r="L6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="52" t="s">
+      <c r="M6" s="15" t="s">
         <v>81</v>
       </c>
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="51"/>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="48"/>
+      <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E7" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="39" t="s">
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="K7" s="39" t="s">
+      <c r="K7" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI7" s="2"/>
     </row>
     <row r="8" spans="1:35">
-      <c r="A8" s="51"/>
-      <c r="B8" s="39" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F8" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="39" t="s">
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H8" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="39" t="s">
+      <c r="H8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L8" s="39" t="s">
+      <c r="L8" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:35">
-      <c r="A9" s="51"/>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="48"/>
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="39" t="s">
+      <c r="F9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="39" t="s">
+      <c r="H9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="6" t="s">
         <v>152</v>
       </c>
       <c r="AI9" s="2"/>
     </row>
     <row r="10" spans="1:35">
-      <c r="A10" s="51"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="K10" s="39" t="s">
+      <c r="K10" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI10" s="2"/>
     </row>
     <row r="11" spans="1:35">
-      <c r="A11" s="51"/>
-      <c r="B11" s="39" t="s">
+      <c r="A11" s="48"/>
+      <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F11" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="39" t="s">
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="39" t="s">
+      <c r="I11" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI11" s="2"/>
     </row>
     <row r="12" spans="1:35">
-      <c r="A12" s="51"/>
-      <c r="B12" s="39" t="s">
+      <c r="A12" s="48"/>
+      <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="F12" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="39" t="s">
+      <c r="F12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="39" t="s">
+      <c r="H12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K12" s="39" t="s">
+      <c r="K12" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="L12" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI12" s="2"/>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" s="51"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F13" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="39" t="s">
+      <c r="F13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="H13" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="39" t="s">
+      <c r="H13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI13" s="2"/>
     </row>
     <row r="14" spans="1:35">
-      <c r="A14" s="51"/>
-      <c r="B14" s="39" t="s">
+      <c r="A14" s="48"/>
+      <c r="B14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="F14" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="39" t="s">
+      <c r="F14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="39" t="s">
+      <c r="H14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="L14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI14" s="2"/>
     </row>
     <row r="15" spans="1:35">
-      <c r="A15" s="51"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="48"/>
+      <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="39" t="s">
+      <c r="F15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="39" t="s">
+      <c r="H15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="M15" s="39" t="s">
+      <c r="M15" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI15" s="2"/>
     </row>
     <row r="16" spans="1:35">
-      <c r="A16" s="51"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="48"/>
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="F16" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="39" t="s">
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="H16" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="39" t="s">
+      <c r="H16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="K16" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="L16" s="39" t="s">
+      <c r="L16" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="M16" s="39" t="s">
+      <c r="M16" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI16" s="2"/>
     </row>
     <row r="17" spans="1:35">
-      <c r="A17" s="51"/>
+      <c r="A17" s="48"/>
       <c r="AI17" s="2"/>
     </row>
     <row r="18" spans="1:35">
-      <c r="A18" s="51"/>
-      <c r="C18" s="48" t="s">
+      <c r="A18" s="48"/>
+      <c r="C18" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="7" t="s">
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M18" s="17" t="s">
         <v>70</v>
       </c>
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="1:35">
-      <c r="A19" s="51"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="A19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
       <c r="AI19" s="2"/>
     </row>
     <row r="20" spans="1:35">
-      <c r="A20" s="51"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="A20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
       <c r="AI20" s="2"/>
     </row>
     <row r="21" spans="1:35" ht="11.25" customHeight="1">
-      <c r="A21" s="51"/>
-      <c r="B21" s="50" t="s">
+      <c r="A21" s="48"/>
+      <c r="B21" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="L21" s="32" t="s">
+      <c r="L21" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="16" t="s">
         <v>202</v>
       </c>
       <c r="AI21" s="2"/>
     </row>
     <row r="22" spans="1:35">
-      <c r="A22" s="51"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="6"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="16"/>
       <c r="AI22" s="2"/>
     </row>
     <row r="23" spans="1:35">
-      <c r="A23" s="51"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="6"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="16"/>
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="1:35">
-      <c r="A24" s="51"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="6"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="16"/>
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="1:35">
-      <c r="A25" s="51"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="6"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="16"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="1:35" s="45" customFormat="1">
-      <c r="A26" s="42"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-    </row>
-    <row r="27" spans="1:35" s="45" customFormat="1">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="40" t="s">
+    <row r="26" spans="1:35" s="12" customFormat="1">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="11"/>
+      <c r="AG26" s="11"/>
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="11"/>
+    </row>
+    <row r="27" spans="1:35" s="12" customFormat="1">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="44"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="44"/>
-      <c r="T27" s="44"/>
-      <c r="U27" s="44"/>
-      <c r="V27" s="44"/>
-      <c r="W27" s="44"/>
-      <c r="X27" s="44"/>
-      <c r="Y27" s="44"/>
-      <c r="Z27" s="44"/>
-      <c r="AA27" s="44"/>
-      <c r="AB27" s="44"/>
-      <c r="AC27" s="44"/>
-      <c r="AD27" s="44"/>
-      <c r="AE27" s="44"/>
-      <c r="AF27" s="44"/>
-      <c r="AG27" s="44"/>
-      <c r="AH27" s="44"/>
-      <c r="AI27" s="44"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="11"/>
+      <c r="AG27" s="11"/>
+      <c r="AH27" s="11"/>
+      <c r="AI27" s="11"/>
     </row>
     <row r="28" spans="1:35" ht="33.75">
-      <c r="M28" s="41" t="s">
+      <c r="M28" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="45" customFormat="1">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="44"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="44"/>
-      <c r="T29" s="44"/>
-      <c r="U29" s="44"/>
-      <c r="V29" s="44"/>
-      <c r="W29" s="44"/>
-      <c r="X29" s="44"/>
-      <c r="Y29" s="44"/>
-      <c r="Z29" s="44"/>
-      <c r="AA29" s="44"/>
-      <c r="AB29" s="44"/>
-      <c r="AC29" s="44"/>
-      <c r="AD29" s="44"/>
-      <c r="AE29" s="44"/>
-      <c r="AF29" s="44"/>
-      <c r="AG29" s="44"/>
-      <c r="AH29" s="44"/>
+    <row r="29" spans="1:35" s="12" customFormat="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="11"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="11"/>
+      <c r="AH29" s="11"/>
     </row>
     <row r="30" spans="1:35" ht="11.25" customHeight="1">
       <c r="C30" s="1"/>
@@ -3337,503 +3337,503 @@
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:35" ht="12.75" customHeight="1">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F32" s="52" t="s">
+      <c r="F32" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="52" t="s">
+      <c r="G32" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H32" s="52" t="s">
+      <c r="H32" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I32" s="52" t="s">
+      <c r="I32" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="J32" s="52" t="s">
+      <c r="J32" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="52" t="s">
+      <c r="K32" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L32" s="52" t="s">
+      <c r="L32" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="M32" s="52" t="s">
+      <c r="M32" s="15" t="s">
         <v>81</v>
       </c>
       <c r="AI32" s="2"/>
     </row>
     <row r="33" spans="1:35">
-      <c r="A33" s="51"/>
-      <c r="B33" s="39" t="s">
+      <c r="A33" s="48"/>
+      <c r="B33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E33" s="39" t="s">
+      <c r="E33" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F33" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" s="39" t="s">
+      <c r="F33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="J33" s="39" t="s">
+      <c r="J33" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="K33" s="39" t="s">
+      <c r="K33" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L33" s="39" t="s">
+      <c r="L33" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M33" s="39" t="s">
+      <c r="M33" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI33" s="2"/>
     </row>
     <row r="34" spans="1:35">
-      <c r="A34" s="51"/>
-      <c r="B34" s="39" t="s">
+      <c r="A34" s="48"/>
+      <c r="B34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E34" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F34" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="39" t="s">
+      <c r="F34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="J34" s="39" t="s">
+      <c r="J34" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K34" s="39" t="s">
+      <c r="K34" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L34" s="39" t="s">
+      <c r="L34" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M34" s="39" t="s">
+      <c r="M34" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI34" s="2"/>
     </row>
     <row r="35" spans="1:35">
-      <c r="A35" s="51"/>
-      <c r="B35" s="39" t="s">
+      <c r="A35" s="48"/>
+      <c r="B35" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E35" s="39" t="s">
+      <c r="E35" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F35" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="39" t="s">
+      <c r="F35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="J35" s="39" t="s">
+      <c r="J35" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K35" s="39" t="s">
+      <c r="K35" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L35" s="39" t="s">
+      <c r="L35" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M35" s="39" t="s">
+      <c r="M35" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AI35" s="2"/>
     </row>
     <row r="36" spans="1:35">
-      <c r="A36" s="51"/>
-      <c r="B36" s="44" t="s">
+      <c r="A36" s="48"/>
+      <c r="B36" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E36" s="44" t="s">
+      <c r="E36" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="F36" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="44" t="s">
+      <c r="F36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="J36" s="44" t="s">
+      <c r="J36" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="K36" s="44" t="s">
+      <c r="K36" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L36" s="44" t="s">
+      <c r="L36" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="M36" s="44" t="s">
+      <c r="M36" s="11" t="s">
         <v>87</v>
       </c>
       <c r="AI36" s="2"/>
     </row>
     <row r="37" spans="1:35">
-      <c r="A37" s="51"/>
-      <c r="B37" s="44" t="s">
+      <c r="A37" s="48"/>
+      <c r="B37" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="44" t="s">
+      <c r="D37" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="44" t="s">
+      <c r="F37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="J37" s="44" t="s">
+      <c r="J37" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="K37" s="44" t="s">
+      <c r="K37" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L37" s="44" t="s">
+      <c r="L37" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="M37" s="44" t="s">
+      <c r="M37" s="11" t="s">
         <v>87</v>
       </c>
       <c r="AI37" s="2"/>
     </row>
     <row r="38" spans="1:35">
-      <c r="A38" s="51"/>
-      <c r="B38" s="44" t="s">
+      <c r="A38" s="48"/>
+      <c r="B38" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F38" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="44" t="s">
+      <c r="F38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="J38" s="44" t="s">
+      <c r="J38" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="K38" s="44" t="s">
+      <c r="K38" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L38" s="44" t="s">
+      <c r="L38" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="M38" s="44" t="s">
+      <c r="M38" s="11" t="s">
         <v>87</v>
       </c>
       <c r="AI38" s="2"/>
     </row>
     <row r="39" spans="1:35">
-      <c r="A39" s="51"/>
-      <c r="B39" s="44" t="s">
+      <c r="A39" s="48"/>
+      <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="44" t="s">
+      <c r="C39" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D39" s="44" t="s">
+      <c r="D39" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E39" s="44" t="s">
+      <c r="E39" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="44" t="s">
+      <c r="F39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="J39" s="44" t="s">
+      <c r="J39" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="K39" s="44" t="s">
+      <c r="K39" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L39" s="44" t="s">
+      <c r="L39" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="M39" s="44" t="s">
+      <c r="M39" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:35">
-      <c r="A40" s="51"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
+      <c r="A40" s="48"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
     </row>
     <row r="41" spans="1:35" ht="13.5" customHeight="1">
-      <c r="A41" s="51"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="53" t="s">
+      <c r="A41" s="48"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="29" t="s">
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="K41" s="29" t="s">
+      <c r="K41" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="M41" s="29" t="s">
+      <c r="M41" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:35" ht="10.5" customHeight="1">
-      <c r="A42" s="51"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="30"/>
+      <c r="A42" s="48"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
     </row>
     <row r="43" spans="1:35" ht="11.25" customHeight="1">
-      <c r="A43" s="51"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
+      <c r="A43" s="48"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
     </row>
     <row r="44" spans="1:35" ht="11.25" customHeight="1">
-      <c r="A44" s="51"/>
-      <c r="B44" s="38" t="s">
+      <c r="A44" s="48"/>
+      <c r="B44" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="E44" s="38" t="s">
+      <c r="E44" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="F44" s="38" t="s">
+      <c r="F44" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="G44" s="38" t="s">
+      <c r="G44" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="H44" s="38" t="s">
+      <c r="H44" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="I44" s="46" t="s">
+      <c r="I44" s="52" t="s">
         <v>208</v>
       </c>
-      <c r="J44" s="32" t="s">
+      <c r="J44" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="K44" s="32" t="s">
+      <c r="K44" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="L44" s="32" t="s">
+      <c r="L44" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="M44" s="32" t="s">
+      <c r="M44" s="23" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
     </row>
     <row r="46" spans="1:35">
-      <c r="A46" s="51"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
-      <c r="L46" s="33"/>
-      <c r="M46" s="33"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
     </row>
     <row r="47" spans="1:35">
-      <c r="A47" s="51"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
     </row>
     <row r="48" spans="1:35">
-      <c r="A48" s="51"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34"/>
+      <c r="A48" s="48"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
     </row>
     <row r="49" spans="2:13">
-      <c r="M49" s="43"/>
+      <c r="M49" s="10"/>
     </row>
     <row r="50" spans="2:13">
-      <c r="M50" s="40" t="s">
+      <c r="M50" s="7" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="51" spans="2:13" ht="33.75">
-      <c r="M51" s="41" t="s">
+      <c r="M51" s="8" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3867,6 +3867,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="L41:L43"/>
+    <mergeCell ref="M21:M25"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="G44:G48"/>
+    <mergeCell ref="H44:H48"/>
+    <mergeCell ref="I44:I48"/>
+    <mergeCell ref="K41:K43"/>
     <mergeCell ref="M41:M43"/>
     <mergeCell ref="K44:K48"/>
     <mergeCell ref="L44:L48"/>
@@ -3883,26 +3903,6 @@
     <mergeCell ref="C44:C48"/>
     <mergeCell ref="D44:D48"/>
     <mergeCell ref="E44:E48"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="G44:G48"/>
-    <mergeCell ref="H44:H48"/>
-    <mergeCell ref="I44:I48"/>
-    <mergeCell ref="K41:K43"/>
-    <mergeCell ref="L41:L43"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="G21:G25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="K21:K25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Mapeamento Conferência LN - EST
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_EST.xlsx
+++ b/Documentação/Planilhas/Conferencia_EST.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="237">
   <si>
     <t>1</t>
   </si>
@@ -695,85 +695,46 @@
     <t>DT_ULT_ATUALIZACAO</t>
   </si>
   <si>
-    <t>101090</t>
-  </si>
-  <si>
-    <t>844.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 11:55:35.000</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>299029</t>
-  </si>
-  <si>
-    <t>887.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 11:53:04.000</t>
-  </si>
-  <si>
-    <t>900000017</t>
-  </si>
-  <si>
-    <t>11402.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 11:42:16.000</t>
-  </si>
-  <si>
-    <t>1736552</t>
-  </si>
-  <si>
-    <t>1978.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 11:28:52.000</t>
-  </si>
-  <si>
-    <t>13422383</t>
-  </si>
-  <si>
-    <t>2014-09-26 11:07:27.000</t>
-  </si>
-  <si>
-    <t>13422384</t>
-  </si>
-  <si>
-    <t>13422427</t>
-  </si>
-  <si>
-    <t>947.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 10:11:22.000</t>
-  </si>
-  <si>
-    <t>1806090</t>
-  </si>
-  <si>
-    <t>13718.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 09:42:47.000</t>
-  </si>
-  <si>
-    <t>1875795</t>
-  </si>
-  <si>
-    <t>2500.0000</t>
-  </si>
-  <si>
-    <t>2014-09-26 09:24:47.000</t>
-  </si>
-  <si>
-    <t>13423608</t>
-  </si>
-  <si>
-    <t>2014-09-25 19:20:02.000</t>
+    <t>2014-07-23 15:09:51.000</t>
+  </si>
+  <si>
+    <t>ALYNE_01</t>
+  </si>
+  <si>
+    <t>995.0000</t>
+  </si>
+  <si>
+    <t>2014-07-23 15:36:39.000</t>
+  </si>
+  <si>
+    <t>ALYNE_02</t>
+  </si>
+  <si>
+    <t>2014-06-30 15:24:28.000</t>
+  </si>
+  <si>
+    <t>50.0000</t>
+  </si>
+  <si>
+    <t>2014-05-15 15:29:03.000</t>
+  </si>
+  <si>
+    <t>32.0000</t>
+  </si>
+  <si>
+    <t>2014-08-04 11:28:58.000</t>
+  </si>
+  <si>
+    <t>1678964</t>
+  </si>
+  <si>
+    <t>2014-03-21 10:06:58.000</t>
+  </si>
+  <si>
+    <t>2013-10-03 15:47:00.000</t>
+  </si>
+  <si>
+    <t>2014-07-11 09:51:09.000</t>
   </si>
 </sst>
 </file>
@@ -1101,6 +1062,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1122,6 +1086,9 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1131,6 +1098,21 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1196,27 +1178,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,19 +1527,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="3" t="s">
         <v>72</v>
       </c>
@@ -1870,106 +1831,106 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:8" ht="11.25" customHeight="1">
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="18"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="18"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="18"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="C26" s="18"/>
+      <c r="C26" s="19"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="C27" s="18"/>
+      <c r="C27" s="19"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="C28" s="18"/>
+      <c r="C28" s="19"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="C29" s="18"/>
+      <c r="C29" s="19"/>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" s="1"/>
-      <c r="C30" s="18"/>
+      <c r="C30" s="19"/>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="1"/>
@@ -2047,25 +2008,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:35" ht="21">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="21">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="32" t="s">
         <v>203</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -2107,7 +2068,7 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="50"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -2147,7 +2108,7 @@
       <c r="AI7" s="2"/>
     </row>
     <row r="8" spans="1:35">
-      <c r="A8" s="50"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -2186,7 +2147,7 @@
       </c>
     </row>
     <row r="9" spans="1:35">
-      <c r="A9" s="50"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
@@ -2226,7 +2187,7 @@
       <c r="AI9" s="2"/>
     </row>
     <row r="10" spans="1:35">
-      <c r="A10" s="50"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
@@ -2266,7 +2227,7 @@
       <c r="AI10" s="2"/>
     </row>
     <row r="11" spans="1:35">
-      <c r="A11" s="50"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
@@ -2306,7 +2267,7 @@
       <c r="AI11" s="2"/>
     </row>
     <row r="12" spans="1:35">
-      <c r="A12" s="50"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
@@ -2346,7 +2307,7 @@
       <c r="AI12" s="2"/>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" s="50"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -2386,7 +2347,7 @@
       <c r="AI13" s="2"/>
     </row>
     <row r="14" spans="1:35">
-      <c r="A14" s="50"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="6" t="s">
         <v>1</v>
       </c>
@@ -2426,7 +2387,7 @@
       <c r="AI14" s="2"/>
     </row>
     <row r="15" spans="1:35">
-      <c r="A15" s="50"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
@@ -2466,7 +2427,7 @@
       <c r="AI15" s="2"/>
     </row>
     <row r="16" spans="1:35">
-      <c r="A16" s="50"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
@@ -2506,162 +2467,162 @@
       <c r="AI16" s="2"/>
     </row>
     <row r="17" spans="1:35">
-      <c r="A17" s="50"/>
+      <c r="A17" s="32"/>
       <c r="AI17" s="2"/>
     </row>
     <row r="18" spans="1:35">
-      <c r="A18" s="50"/>
-      <c r="C18" s="51" t="s">
+      <c r="A18" s="32"/>
+      <c r="C18" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="19" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="M18" s="20" t="s">
         <v>215</v>
       </c>
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="1:35">
-      <c r="A19" s="50"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
+      <c r="A19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
       <c r="AI19" s="2"/>
     </row>
     <row r="20" spans="1:35">
-      <c r="A20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
+      <c r="A20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
       <c r="AI20" s="2"/>
     </row>
     <row r="21" spans="1:35" ht="11.25" customHeight="1">
-      <c r="A21" s="50"/>
-      <c r="B21" s="55" t="s">
+      <c r="A21" s="32"/>
+      <c r="B21" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="L21" s="25" t="s">
+      <c r="L21" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="M21" s="18" t="s">
+      <c r="M21" s="19" t="s">
         <v>199</v>
       </c>
       <c r="AI21" s="2"/>
     </row>
     <row r="22" spans="1:35">
-      <c r="A22" s="50"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="18"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="19"/>
       <c r="AI22" s="2"/>
     </row>
     <row r="23" spans="1:35">
-      <c r="A23" s="50"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="18"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="19"/>
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="1:35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="18"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="19"/>
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="1:35">
-      <c r="A25" s="50"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="18"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="19"/>
       <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="1:35" s="12" customFormat="1">
@@ -2808,7 +2769,7 @@
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:35" ht="12.75" customHeight="1">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="32" t="s">
         <v>204</v>
       </c>
       <c r="B32" s="15" t="s">
@@ -2850,7 +2811,7 @@
       <c r="AI32" s="2"/>
     </row>
     <row r="33" spans="1:35">
-      <c r="A33" s="50"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="6" t="s">
         <v>1</v>
       </c>
@@ -2890,7 +2851,7 @@
       <c r="AI33" s="2"/>
     </row>
     <row r="34" spans="1:35">
-      <c r="A34" s="50"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="6" t="s">
         <v>1</v>
       </c>
@@ -2930,7 +2891,7 @@
       <c r="AI34" s="2"/>
     </row>
     <row r="35" spans="1:35">
-      <c r="A35" s="50"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="6" t="s">
         <v>1</v>
       </c>
@@ -2970,7 +2931,7 @@
       <c r="AI35" s="2"/>
     </row>
     <row r="36" spans="1:35">
-      <c r="A36" s="50"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="11" t="s">
         <v>1</v>
       </c>
@@ -3010,7 +2971,7 @@
       <c r="AI36" s="2"/>
     </row>
     <row r="37" spans="1:35">
-      <c r="A37" s="50"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="11" t="s">
         <v>1</v>
       </c>
@@ -3050,7 +3011,7 @@
       <c r="AI37" s="2"/>
     </row>
     <row r="38" spans="1:35">
-      <c r="A38" s="50"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="11" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3051,7 @@
       <c r="AI38" s="2"/>
     </row>
     <row r="39" spans="1:35">
-      <c r="A39" s="50"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
@@ -3129,7 +3090,7 @@
       </c>
     </row>
     <row r="40" spans="1:35">
-      <c r="A40" s="50"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -3144,156 +3105,156 @@
       <c r="M40" s="11"/>
     </row>
     <row r="41" spans="1:35" ht="13.5" customHeight="1">
-      <c r="A41" s="50"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="22" t="s">
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="K41" s="22" t="s">
+      <c r="K41" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="22" t="s">
+      <c r="L41" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="M41" s="22" t="s">
+      <c r="M41" s="23" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:35" ht="10.5" customHeight="1">
-      <c r="A42" s="50"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
+      <c r="A42" s="32"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
     </row>
     <row r="43" spans="1:35" ht="11.25" customHeight="1">
-      <c r="A43" s="50"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
+      <c r="A43" s="32"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
     </row>
     <row r="44" spans="1:35" ht="11.25" customHeight="1">
-      <c r="A44" s="50"/>
-      <c r="B44" s="53" t="s">
+      <c r="A44" s="32"/>
+      <c r="B44" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="53" t="s">
+      <c r="C44" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="D44" s="53" t="s">
+      <c r="D44" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="E44" s="53" t="s">
+      <c r="E44" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="F44" s="53" t="s">
+      <c r="F44" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="G44" s="53" t="s">
+      <c r="G44" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="H44" s="53" t="s">
+      <c r="H44" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="I44" s="54" t="s">
+      <c r="I44" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="J44" s="25" t="s">
+      <c r="J44" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="K44" s="25" t="s">
+      <c r="K44" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="L44" s="25" t="s">
+      <c r="L44" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="M44" s="25" t="s">
+      <c r="M44" s="27" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:35">
-      <c r="A45" s="50"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
     </row>
     <row r="46" spans="1:35">
-      <c r="A46" s="50"/>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
     </row>
     <row r="47" spans="1:35">
-      <c r="A47" s="50"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
     </row>
     <row r="48" spans="1:35">
-      <c r="A48" s="50"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
     </row>
     <row r="49" spans="2:13">
       <c r="M49" s="10"/>
@@ -3338,6 +3299,27 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="M44:M48"/>
+    <mergeCell ref="A6:A25"/>
+    <mergeCell ref="C18:K20"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="A32:A48"/>
+    <mergeCell ref="C41:I43"/>
+    <mergeCell ref="J41:J43"/>
+    <mergeCell ref="J44:J48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="G44:G48"/>
+    <mergeCell ref="H44:H48"/>
+    <mergeCell ref="I44:I48"/>
+    <mergeCell ref="K41:K43"/>
+    <mergeCell ref="K44:K48"/>
+    <mergeCell ref="L41:L43"/>
+    <mergeCell ref="L44:L48"/>
     <mergeCell ref="M41:M43"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -3353,27 +3335,6 @@
     <mergeCell ref="H21:H25"/>
     <mergeCell ref="J21:J25"/>
     <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H44:H48"/>
-    <mergeCell ref="I44:I48"/>
-    <mergeCell ref="K41:K43"/>
-    <mergeCell ref="K44:K48"/>
-    <mergeCell ref="L41:L43"/>
-    <mergeCell ref="L44:L48"/>
-    <mergeCell ref="M44:M48"/>
-    <mergeCell ref="A6:A25"/>
-    <mergeCell ref="C18:K20"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="A32:A48"/>
-    <mergeCell ref="C41:I43"/>
-    <mergeCell ref="J41:J43"/>
-    <mergeCell ref="J44:J48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="E44:E48"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="G44:G48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3429,19 +3390,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="3" t="s">
         <v>136</v>
       </c>
@@ -3816,188 +3777,181 @@
       <c r="AH18" s="1"/>
     </row>
     <row r="19" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="41" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="22" t="s">
+      <c r="G19" s="49"/>
+      <c r="H19" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="23" t="s">
         <v>219</v>
       </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
     <row r="20" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
     <row r="21" spans="1:34" ht="11.25" customHeight="1">
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
     <row r="22" spans="1:34" ht="11.25" customHeight="1">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="I22" s="47" t="s">
+      <c r="I22" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="36" t="s">
         <v>121</v>
       </c>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
     <row r="23" spans="1:34">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="30"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="37"/>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="30"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="37"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="30"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="37"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="30"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="37"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="J27" s="30"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="35" t="s">
         <v>130</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="J28" s="30"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:34" ht="33.75">
-      <c r="D29" s="28"/>
+      <c r="D29" s="35"/>
       <c r="F29" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="J29" s="30"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:34">
-      <c r="D30" s="28"/>
+      <c r="D30" s="35"/>
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="J30" s="30"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="1:34">
-      <c r="J31" s="30"/>
+      <c r="J31" s="37"/>
     </row>
     <row r="32" spans="1:34">
-      <c r="J32" s="30"/>
+      <c r="J32" s="37"/>
     </row>
     <row r="33" spans="10:10">
-      <c r="J33" s="30"/>
+      <c r="J33" s="37"/>
     </row>
     <row r="34" spans="10:10">
-      <c r="J34" s="31"/>
+      <c r="J34" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="J22:J34"/>
-    <mergeCell ref="B19:E21"/>
-    <mergeCell ref="F19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I22:I26"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="J19:J21"/>
@@ -4009,6 +3963,13 @@
     <mergeCell ref="G22:G26"/>
     <mergeCell ref="D22:D26"/>
     <mergeCell ref="B22:B26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="J22:J34"/>
+    <mergeCell ref="B19:E21"/>
+    <mergeCell ref="F19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4023,7 +3984,7 @@
   <dimension ref="A2:AH26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C26:C27"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -4066,44 +4027,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="3"/>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1">
       <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="18" t="s">
         <v>30</v>
       </c>
       <c r="J6" s="17"/>
@@ -4113,22 +4074,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>149</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4136,22 +4097,22 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>149</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4159,22 +4120,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>149</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>231</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4182,22 +4143,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>233</v>
+        <v>146</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>234</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4205,22 +4166,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>236</v>
+        <v>84</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>143</v>
+        <v>231</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>226</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -4228,22 +4189,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -4251,22 +4212,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>239</v>
+        <v>93</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>240</v>
+        <v>94</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>226</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -4274,22 +4235,22 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>242</v>
+        <v>98</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>243</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>226</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -4297,22 +4258,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>187</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>188</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>245</v>
+        <v>101</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>246</v>
+        <v>61</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>226</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -4320,43 +4281,43 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>248</v>
+        <v>103</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>226</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="53"/>
+      <c r="A22" s="30"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="53"/>
+      <c r="A23" s="30"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="53"/>
+      <c r="A24" s="30"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="53"/>
+      <c r="A25" s="30"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="53"/>
+      <c r="A26" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4374,13 +4335,13 @@
   <dimension ref="C3:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F14"/>
+      <selection activeCell="F3" sqref="F3:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:6">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="str">
@@ -4389,57 +4350,57 @@
       </c>
     </row>
     <row r="4" spans="3:6">
-      <c r="C4" s="4" t="s">
-        <v>15</v>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F48" si="0">CONCATENATE(C4,",")</f>
-        <v>CD_ITEM,</v>
+        <v>CD_UNIDADE_EMPRESARIAL,</v>
       </c>
     </row>
     <row r="5" spans="3:6">
-      <c r="C5" s="4" t="s">
-        <v>78</v>
+      <c r="C5" s="18" t="s">
+        <v>6</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>CD_DEPOSITO,</v>
+        <v>CD_FILIAL,</v>
       </c>
     </row>
     <row r="6" spans="3:6">
-      <c r="C6" s="4" t="s">
-        <v>80</v>
+      <c r="C6" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>QT_FISICA,</v>
+        <v>CD_ITEM,</v>
       </c>
     </row>
     <row r="7" spans="3:6">
-      <c r="C7" s="4" t="s">
-        <v>138</v>
+      <c r="C7" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>QT_ROMANEADA,</v>
+        <v>QT_FISICA,</v>
       </c>
     </row>
     <row r="8" spans="3:6">
-      <c r="C8" s="4" t="s">
-        <v>51</v>
+      <c r="C8" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>QT_SALDO,</v>
+        <v>DT_ULT_ATUALIZACAO,</v>
       </c>
     </row>
     <row r="9" spans="3:6">
-      <c r="C9" s="4" t="s">
-        <v>49</v>
+      <c r="C9" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>QT_RESERVADA,</v>
+        <v>VL_CMV,</v>
       </c>
     </row>
     <row r="10" spans="3:6">

</xml_diff>